<commit_message>
overhaul of whole project
</commit_message>
<xml_diff>
--- a/Summary table.xlsx
+++ b/Summary table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t xml:space="preserve">Training data setup</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t xml:space="preserve">Model performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test fraction in subvolumes/windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test fraction in number of eyes/scans</t>
   </si>
   <si>
     <t xml:space="preserve">Fiddler Crab</t>
@@ -82,6 +88,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -103,6 +110,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -277,21 +285,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.21"/>
   </cols>
@@ -341,35 +349,49 @@
       <c r="H3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="8"/>
+      <c r="I3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="9" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>557</v>
+        <v>156</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="10" t="n">
-        <v>36</v>
+        <v>2</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="0" t="n">
+        <f aca="false">G4/(G4+D4)</f>
+        <v>0.287671232876712</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">F4/(F4+C4)</f>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="9"/>
       <c r="E5" s="10"/>
@@ -404,22 +426,22 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added summary of data
</commit_message>
<xml_diff>
--- a/Summary table.xlsx
+++ b/Summary table.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t xml:space="preserve">Training data setup</t>
   </si>
@@ -74,6 +75,36 @@
   </si>
   <si>
     <t xml:space="preserve">To reduce the impact of incompletely annotated data, I could try loading the volume and annotations, then cropping to the edge of the annotations, and then chopping up the volume into subvolumes/windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiddler crab model training data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dampieri_20151218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dampieri_male_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dampieri_20200218_male_left_1676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flammula_20190925_male_left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flammula_20180307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flammula_20200327_female_left_178_fullres_cropped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paraphronima model training data</t>
   </si>
 </sst>
 </file>
@@ -287,11 +318,11 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.72"/>
@@ -459,4 +490,84 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>